<commit_message>
new updates + history page
</commit_message>
<xml_diff>
--- a/dashboardWebsite/backend/uploads/PO.xlsx
+++ b/dashboardWebsite/backend/uploads/PO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8C1580-E567-B346-B1D2-1349234485A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC729C56-61B0-8342-9B1D-72279D564944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3080" yWindow="2120" windowWidth="28040" windowHeight="17440" xr2:uid="{821E3D18-53EE-3F49-ACED-58A0260C8EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>PO</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -432,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24281A0-A111-8343-B54B-5906E5D39EA8}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,6 +516,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45737</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45737</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>